<commit_message>
removed unnecesary data for the purpose
</commit_message>
<xml_diff>
--- a/files/experimentResults/Results SUS plugin.xlsx
+++ b/files/experimentResults/Results SUS plugin.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Participant\Question</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>10. I needed to learn a lot of things before I could get going with the plugin.</t>
-  </si>
-  <si>
-    <t>PILOT</t>
   </si>
   <si>
     <t>P1</t>
@@ -363,16 +360,16 @@
         <v>11</v>
       </c>
       <c r="B2" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C2" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D2" s="1">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="E2" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="F2" s="1">
         <v>4.0</v>
@@ -384,13 +381,13 @@
         <v>4.0</v>
       </c>
       <c r="I2" s="1">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="J2" s="1">
         <v>4.0</v>
       </c>
       <c r="K2" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
@@ -398,34 +395,34 @@
         <v>12</v>
       </c>
       <c r="B3" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C3" s="1">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D3" s="1">
         <v>3.0</v>
       </c>
       <c r="E3" s="1">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="F3" s="1">
         <v>4.0</v>
       </c>
       <c r="G3" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H3" s="1">
         <v>4.0</v>
       </c>
       <c r="I3" s="1">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="J3" s="1">
         <v>4.0</v>
       </c>
       <c r="K3" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="4">
@@ -436,31 +433,31 @@
         <v>4.0</v>
       </c>
       <c r="C4" s="1">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D4" s="1">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="E4" s="1">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="F4" s="1">
         <v>4.0</v>
       </c>
       <c r="G4" s="1">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H4" s="1">
         <v>4.0</v>
       </c>
       <c r="I4" s="1">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="J4" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="K4" s="1">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
@@ -474,28 +471,28 @@
         <v>2.0</v>
       </c>
       <c r="D5" s="1">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="E5" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="F5" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="G5" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H5" s="1">
         <v>4.0</v>
       </c>
       <c r="I5" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="J5" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="K5" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="6">
@@ -509,16 +506,16 @@
         <v>2.0</v>
       </c>
       <c r="D6" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E6" s="1">
         <v>2.0</v>
       </c>
       <c r="F6" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G6" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H6" s="1">
         <v>4.0</v>
@@ -530,41 +527,6 @@
         <v>4.0</v>
       </c>
       <c r="K6" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="H7" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="J7" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="K7" s="1">
         <v>2.0</v>
       </c>
     </row>

</xml_diff>